<commit_message>
Plantable Stack Dummy Data First Cut
</commit_message>
<xml_diff>
--- a/Data/DummyData_Harford.xlsx
+++ b/Data/DummyData_Harford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbouf\Documents\UVM\Maryland_Technical_Forest\MD_Forest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4A97FB-440A-4969-95B4-FC67B9F0B635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5A1AAC-9CC3-44E0-930C-55DE6B62020B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C25"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,11 +525,11 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">F2*I2</f>
-        <v>535517526.13413858</v>
+        <v>463089476.33328086</v>
       </c>
       <c r="C2" s="1">
         <f ca="1">D2*J2</f>
-        <v>135012076.08980122</v>
+        <v>145298852.62611827</v>
       </c>
       <c r="D2">
         <v>115054502</v>
@@ -546,15 +546,15 @@
       </c>
       <c r="H2">
         <f ca="1">RAND()*(0.35-0.1)+0.1</f>
-        <v>0.17346191363986108</v>
+        <v>0.26286977128559708</v>
       </c>
       <c r="I2">
         <f ca="1">RAND()*(0.7-0.35)+0.35</f>
-        <v>0.48972769971964725</v>
+        <v>0.42349266446280032</v>
       </c>
       <c r="J2">
         <f ca="1">1+H2</f>
-        <v>1.1734619136398612</v>
+        <v>1.262869771285597</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -562,12 +562,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B25" ca="1" si="0">F3*I3</f>
-        <v>526143162.20429373</v>
+        <f t="shared" ref="B3:C26" ca="1" si="0">F3*I3</f>
+        <v>578905325.04974532</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C13" ca="1" si="1">D3*J3</f>
-        <v>204078354.11551324</v>
+        <f t="shared" ref="C3:C12" ca="1" si="1">D3*J3</f>
+        <v>237781143.96834174</v>
       </c>
       <c r="D3">
         <v>180174673</v>
@@ -584,15 +584,15 @@
       </c>
       <c r="H3" s="3">
         <f t="shared" ref="H3:H25" ca="1" si="3">RAND()*(0.35-0.1)+0.1</f>
-        <v>0.13266948521401359</v>
+        <v>0.31972568624193776</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I13" ca="1" si="4">RAND()*(0.7-0.35)+0.35</f>
-        <v>0.49441292573819912</v>
+        <v>0.54399314871668591</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" ref="J3:J25" ca="1" si="5">1+H3</f>
-        <v>1.1326694852140136</v>
+        <v>1.3197256862419378</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -601,11 +601,11 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>689099213.9696697</v>
+        <v>777528744.79065669</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>411021061.87273914</v>
+        <v>440334962.33325571</v>
       </c>
       <c r="D4">
         <v>355198713</v>
@@ -622,15 +622,15 @@
       </c>
       <c r="H4" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.1571580831508787</v>
+        <v>0.23968625509421737</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="4"/>
-        <v>0.44702832616589405</v>
+        <v>0.50439380321936378</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1571580831508788</v>
+        <v>1.2396862550942174</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -639,11 +639,11 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>92513234.720594287</v>
+        <v>113801728.75846665</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>51105848.836137868</v>
+        <v>50506847.634041578</v>
       </c>
       <c r="D5">
         <v>38266532</v>
@@ -660,15 +660,15 @@
       </c>
       <c r="H5" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.33552339773402684</v>
+        <v>0.31987000112896508</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="4"/>
-        <v>0.44259807720203603</v>
+        <v>0.54444562967543186</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.3355233977340268</v>
+        <v>1.319870001128965</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -677,11 +677,11 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>283986175.41162169</v>
+        <v>197975064.546175</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>97991027.425451398</v>
+        <v>104273295.69966178</v>
       </c>
       <c r="D6">
         <v>79220030</v>
@@ -698,15 +698,15 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23694761824063179</v>
+        <v>0.31624913168628921</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.51507768777792995</v>
+        <v>0.35907571323261389</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2369476182406318</v>
+        <v>1.3162491316862892</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -715,11 +715,11 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>302732236.4914366</v>
+        <v>441831090.66784644</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>91953060.533729658</v>
+        <v>105349472.64578553</v>
       </c>
       <c r="D7">
         <v>78706398</v>
@@ -736,15 +736,15 @@
       </c>
       <c r="H7" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16830477407604971</v>
+        <v>0.33851218354301416</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="4"/>
-        <v>0.36784082582113969</v>
+        <v>0.53685565550701697</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1683047740760497</v>
+        <v>1.3385121835430143</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -753,11 +753,11 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>569634835.26008618</v>
+        <v>607346749.16341913</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>250719605.03895992</v>
+        <v>222054939.73618388</v>
       </c>
       <c r="D8">
         <v>197293958</v>
@@ -774,15 +774,15 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.27079210929997127</v>
+        <v>0.12550299049798511</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.49115039080107825</v>
+        <v>0.52366634682231006</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2707921092999712</v>
+        <v>1.1255029904979852</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -791,11 +791,11 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>343209267.46333593</v>
+        <v>371354424.14821732</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>179216924.53180039</v>
+        <v>191787955.83817375</v>
       </c>
       <c r="D9">
         <v>156318101</v>
@@ -812,15 +812,15 @@
       </c>
       <c r="H9" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14648862406408325</v>
+        <v>0.22690817385360734</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="4"/>
-        <v>0.38382064180445757</v>
+        <v>0.41529616745771575</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1464886240640833</v>
+        <v>1.2269081738536074</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -829,11 +829,11 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>688226005.19404614</v>
+        <v>496327758.90780437</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>213004034.88840541</v>
+        <v>223076726.45122313</v>
       </c>
       <c r="D10">
         <v>174019757</v>
@@ -850,15 +850,15 @@
       </c>
       <c r="H10" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22402213725884818</v>
+        <v>0.28190459690863223</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="4"/>
-        <v>0.58261671358799838</v>
+        <v>0.42016553512218691</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2240221372588482</v>
+        <v>1.2819045969086322</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -867,11 +867,11 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>862186549.6172241</v>
+        <v>493668228.45555067</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>106594310.10303414</v>
+        <v>106294075.22050008</v>
       </c>
       <c r="D11">
         <v>89256965</v>
@@ -888,15 +888,15 @@
       </c>
       <c r="H11" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19424080914059921</v>
+        <v>0.19087709536729247</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="4"/>
-        <v>0.63112255034837761</v>
+        <v>0.36136628610960697</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1942408091405992</v>
+        <v>1.1908770953672925</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -905,11 +905,11 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>749564167.42617643</v>
+        <v>673044315.05037344</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>296595292.76029122</v>
+        <v>339903628.31055504</v>
       </c>
       <c r="D12">
         <v>260948788</v>
@@ -926,15 +926,15 @@
       </c>
       <c r="H12" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13660345017694123</v>
+        <v>0.30256833501964775</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="4"/>
-        <v>0.43846529661743405</v>
+        <v>0.39370421914452619</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1366034501769413</v>
+        <v>1.3025683350196477</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -943,11 +943,11 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>896629139.80161309</v>
+        <v>945153295.53206539</v>
       </c>
       <c r="C13" s="1">
         <f ca="1">D13*J13</f>
-        <v>249484352.19157577</v>
+        <v>249896156.97702202</v>
       </c>
       <c r="D13">
         <v>216988249</v>
@@ -964,15 +964,15 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14975973741129056</v>
+        <v>0.15165755808749806</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="4"/>
-        <v>0.53533293053174758</v>
+        <v>0.56430430491124794</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1497597374112907</v>
+        <v>1.1516575580874981</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>230392387.23486295</v>
+        <v>276459176.59027654</v>
       </c>
       <c r="C15" s="1">
         <f>D15*J15</f>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="I15">
         <f ca="1">RAND()*(0.7-0.35)+0.35</f>
-        <v>0.35537700616304746</v>
+        <v>0.42643437867936196</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="5"/>
@@ -1043,11 +1043,11 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>285376193.95102817</v>
+        <v>315486012.0996303</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ref="C16:C25" ca="1" si="6">D16*J16</f>
-        <v>97413057.125711545</v>
+        <v>108343564.76386534</v>
       </c>
       <c r="D16">
         <v>82895775</v>
@@ -1064,15 +1064,15 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.17512692445075217</v>
+        <v>0.30698536522356346</v>
       </c>
       <c r="I16">
         <f t="shared" ref="I16:I25" ca="1" si="7">RAND()*(0.7-0.35)+0.35</f>
-        <v>0.40119302291671877</v>
+        <v>0.44352258375101639</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1751269244507521</v>
+        <v>1.3069853652235635</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1081,11 +1081,11 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>842928070.94779885</v>
+        <v>641433143.34267211</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>383876110.86815095</v>
+        <v>416152889.10505432</v>
       </c>
       <c r="D17">
         <v>314717229</v>
@@ -1102,15 +1102,15 @@
       </c>
       <c r="H17" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.21974927171257913</v>
+        <v>0.32230729924561685</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.65980968551235408</v>
+        <v>0.50208768123032266</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2197492717125791</v>
+        <v>1.3223072992456169</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1119,11 +1119,11 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>500865767.95872688</v>
+        <v>556412081.82920003</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>367770233.55304068</v>
+        <v>391113851.00444841</v>
       </c>
       <c r="D18">
         <v>289754271</v>
@@ -1140,15 +1140,15 @@
       </c>
       <c r="H18" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.26924870609772883</v>
+        <v>0.34981220347377862</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="7"/>
-        <v>0.40240481401437989</v>
+        <v>0.44703174907789572</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2692487060977289</v>
+        <v>1.3498122034737787</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1157,11 +1157,11 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>572771159.11710596</v>
+        <v>510631633.75489783</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>136316739.67930177</v>
+        <v>124528818.84608179</v>
       </c>
       <c r="D19">
         <v>110232774</v>
@@ -1178,15 +1178,15 @@
       </c>
       <c r="H19" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23662622950323084</v>
+        <v>0.12968960434654217</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="7"/>
-        <v>0.60210221319247137</v>
+        <v>0.53678058316314647</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2366262295032309</v>
+        <v>1.1296896043465421</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1195,11 +1195,11 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>323325690.61866736</v>
+        <v>341467500.191369</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>38131904.113664798</v>
+        <v>38509884.772157244</v>
       </c>
       <c r="D20">
         <v>33286617</v>
@@ -1216,15 +1216,15 @@
       </c>
       <c r="H20" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14556261796339356</v>
+        <v>0.15691795210541365</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="7"/>
-        <v>0.40162243822091942</v>
+        <v>0.4241574795298434</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1455626179633935</v>
+        <v>1.1569179521054136</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1233,11 +1233,11 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>514409446.66137135</v>
+        <v>585889362.00708771</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>160846222.08729398</v>
+        <v>157268099.67072079</v>
       </c>
       <c r="D21">
         <v>131644727</v>
@@ -1254,15 +1254,15 @@
       </c>
       <c r="H21" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.2218204690210947</v>
+        <v>0.19464032669322762</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="7"/>
-        <v>0.55821513263096201</v>
+        <v>0.63578207990249092</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2218204690210948</v>
+        <v>1.1946403266932277</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1271,11 +1271,11 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>369799654.92044538</v>
+        <v>410780372.40378678</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>66428130.85089305</v>
+        <v>71336778.737800315</v>
       </c>
       <c r="D22">
         <v>56024738</v>
@@ -1292,15 +1292,15 @@
       </c>
       <c r="H22" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18569284252419088</v>
+        <v>0.27330856483077737</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="7"/>
-        <v>0.53928629596236377</v>
+        <v>0.59904930288627689</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1856928425241908</v>
+        <v>1.2733085648307774</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>801361871.80022907</v>
+        <v>510252608.17612278</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="6"/>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="7"/>
-        <v>0.68106744603274572</v>
+        <v>0.4336573187608449</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" si="5"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>574237447.12167013</v>
+        <v>507397008.3855744</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="6"/>
@@ -1370,7 +1370,7 @@
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="7"/>
-        <v>0.59756929661941605</v>
+        <v>0.52801306311101692</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" si="5"/>
@@ -1383,11 +1383,11 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>450129625.44473106</v>
+        <v>518498812.25827289</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>153907782.34805855</v>
+        <v>166698450.64749473</v>
       </c>
       <c r="D25">
         <v>134544096</v>
@@ -1404,16 +1404,26 @@
       </c>
       <c r="H25" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14392074363529522</v>
+        <v>0.23898748145362511</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="7"/>
-        <v>0.37704657474745873</v>
+        <v>0.43431533967455249</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1439207436352952</v>
-      </c>
+        <v>1.238987481453625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.35">
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.35">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tweak plantable percent legend
</commit_message>
<xml_diff>
--- a/Data/DummyData_Harford.xlsx
+++ b/Data/DummyData_Harford.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbouf\Documents\UVM\Maryland_Technical_Forest\MD_Forest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5A1AAC-9CC3-44E0-930C-55DE6B62020B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC45544-1497-4528-BC61-F2FD40C504E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,7 +135,7 @@
     <t>Percent Increase</t>
   </si>
   <si>
-    <t>Random Number (10-25)</t>
+    <t>Random Number (15-45)</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,11 +525,11 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">F2*I2</f>
-        <v>463089476.33328086</v>
+        <v>487885194.60957557</v>
       </c>
       <c r="C2" s="1">
         <f ca="1">D2*J2</f>
-        <v>145298852.62611827</v>
+        <v>154807436.55944127</v>
       </c>
       <c r="D2">
         <v>115054502</v>
@@ -545,16 +545,16 @@
         <v>0.1052166807940025</v>
       </c>
       <c r="H2">
-        <f ca="1">RAND()*(0.35-0.1)+0.1</f>
-        <v>0.26286977128559708</v>
+        <f ca="1">RAND()*(0.45-0.15)+0.15</f>
+        <v>0.3455139422483553</v>
       </c>
       <c r="I2">
         <f ca="1">RAND()*(0.7-0.35)+0.35</f>
-        <v>0.42349266446280032</v>
+        <v>0.44616820631108811</v>
       </c>
       <c r="J2">
         <f ca="1">1+H2</f>
-        <v>1.262869771285597</v>
+        <v>1.3455139422483553</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -562,12 +562,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:C26" ca="1" si="0">F3*I3</f>
-        <v>578905325.04974532</v>
+        <f t="shared" ref="B3:C27" ca="1" si="0">F3*I3</f>
+        <v>674121260.69472599</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C12" ca="1" si="1">D3*J3</f>
-        <v>237781143.96834174</v>
+        <v>236426490.96150044</v>
       </c>
       <c r="D3">
         <v>180174673</v>
@@ -583,16 +583,16 @@
         <v>0.1693088376339377</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H25" ca="1" si="3">RAND()*(0.35-0.1)+0.1</f>
-        <v>0.31972568624193776</v>
+        <f t="shared" ref="H3:H25" ca="1" si="3">RAND()*(0.45-0.15)+0.15</f>
+        <v>0.31220713225049368</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I13" ca="1" si="4">RAND()*(0.7-0.35)+0.35</f>
-        <v>0.54399314871668591</v>
+        <v>0.63346687507266208</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" ref="J3:J25" ca="1" si="5">1+H3</f>
-        <v>1.3197256862419378</v>
+        <v>1.3122071322504936</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -601,11 +601,11 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>777528744.79065669</v>
+        <v>570293746.50289905</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>440334962.33325571</v>
+        <v>408964777.26701248</v>
       </c>
       <c r="D4">
         <v>355198713</v>
@@ -622,15 +622,15 @@
       </c>
       <c r="H4" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23968625509421737</v>
+        <v>0.15136897263198268</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="4"/>
-        <v>0.50439380321936378</v>
+        <v>0.36995755292399535</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2396862550942174</v>
+        <v>1.1513689726319827</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -639,11 +639,11 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>113801728.75846665</v>
+        <v>141658914.88983974</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>50506847.634041578</v>
+        <f t="shared" si="1"/>
+        <v>47833165</v>
       </c>
       <c r="D5">
         <v>38266532</v>
@@ -659,16 +659,15 @@
         <v>0.18307319526273055</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.31987000112896508</v>
+        <v>0.25</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="4"/>
-        <v>0.54444562967543186</v>
+        <v>0.67771885328762371</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" ca="1" si="5"/>
-        <v>1.319870001128965</v>
+        <f t="shared" si="5"/>
+        <v>1.25</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -677,11 +676,11 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>197975064.546175</v>
+        <v>195604457.31628919</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>104273295.69966178</v>
+        <v>112648690.59895995</v>
       </c>
       <c r="D6">
         <v>79220030</v>
@@ -698,15 +697,15 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.31624913168628921</v>
+        <v>0.42197232945960683</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="4"/>
-        <v>0.35907571323261389</v>
+        <v>0.35477604305032634</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.3162491316862892</v>
+        <v>1.4219723294596069</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -715,11 +714,11 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>441831090.66784644</v>
+        <v>561460287.57249415</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>105349472.64578553</v>
+        <v>109620293.1624583</v>
       </c>
       <c r="D7">
         <v>78706398</v>
@@ -736,15 +735,15 @@
       </c>
       <c r="H7" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.33851218354301416</v>
+        <v>0.39277486898153169</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="4"/>
-        <v>0.53685565550701697</v>
+        <v>0.68221349083939686</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.3385121835430143</v>
+        <v>1.3927748689815318</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -753,11 +752,11 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>607346749.16341913</v>
+        <v>537632244.83191121</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>222054939.73618388</v>
+        <v>260965383.9451057</v>
       </c>
       <c r="D8">
         <v>197293958</v>
@@ -774,15 +773,15 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.12550299049798511</v>
+        <v>0.32272364846117446</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.52366634682231006</v>
+        <v>0.46355712609445554</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1255029904979852</v>
+        <v>1.3227236484611744</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -791,11 +790,11 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>371354424.14821732</v>
+        <v>334404690.71320266</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>191787955.83817375</v>
+        <v>212992566.92280772</v>
       </c>
       <c r="D9">
         <v>156318101</v>
@@ -812,15 +811,15 @@
       </c>
       <c r="H9" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.22690817385360734</v>
+        <v>0.36255856206190562</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="4"/>
-        <v>0.41529616745771575</v>
+        <v>0.37397423432242832</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2269081738536074</v>
+        <v>1.3625585620619056</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -829,11 +828,11 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>496327758.90780437</v>
+        <v>434725868.08448482</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>223076726.45122313</v>
+        <v>232851804.06401929</v>
       </c>
       <c r="D10">
         <v>174019757</v>
@@ -850,15 +849,15 @@
       </c>
       <c r="H10" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.28190459690863223</v>
+        <v>0.33807682574812059</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="4"/>
-        <v>0.42016553512218691</v>
+        <v>0.36801654494828351</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2819045969086322</v>
+        <v>1.3380768257481206</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -867,11 +866,11 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>493668228.45555067</v>
+        <v>503356935.00746596</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>106294075.22050008</v>
+        <v>108453560.25327517</v>
       </c>
       <c r="D11">
         <v>89256965</v>
@@ -888,15 +887,15 @@
       </c>
       <c r="H11" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19087709536729247</v>
+        <v>0.21507111801611423</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="4"/>
-        <v>0.36136628610960697</v>
+        <v>0.36845844173571424</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1908770953672925</v>
+        <v>1.2150711180161142</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -905,11 +904,11 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>673044315.05037344</v>
+        <v>798293279.74779487</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>339903628.31055504</v>
+        <v>326696510.58754158</v>
       </c>
       <c r="D12">
         <v>260948788</v>
@@ -926,15 +925,15 @@
       </c>
       <c r="H12" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.30256833501964775</v>
+        <v>0.25195642061208412</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="4"/>
-        <v>0.39370421914452619</v>
+        <v>0.46696989384407106</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.3025683350196477</v>
+        <v>1.2519564206120841</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -943,11 +942,11 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>945153295.53206539</v>
+        <v>932686186.39469242</v>
       </c>
       <c r="C13" s="1">
         <f ca="1">D13*J13</f>
-        <v>249896156.97702202</v>
+        <v>296977857.59940988</v>
       </c>
       <c r="D13">
         <v>216988249</v>
@@ -964,15 +963,15 @@
       </c>
       <c r="H13" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15165755808749806</v>
+        <v>0.36863567021737609</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="4"/>
-        <v>0.56430430491124794</v>
+        <v>0.5568608104122339</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1516575580874981</v>
+        <v>1.3686356702173761</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1006,11 +1005,11 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>276459176.59027654</v>
+        <v>332180515.20723885</v>
       </c>
       <c r="C15" s="1">
-        <f>D15*J15</f>
-        <v>177662296.00000003</v>
+        <f ca="1">D15*J15</f>
+        <v>190433374.83200073</v>
       </c>
       <c r="D15">
         <v>158627050</v>
@@ -1026,15 +1025,16 @@
         <v>0.24467998618378731</v>
       </c>
       <c r="H15" s="3">
-        <v>0.12</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.20051009479152965</v>
       </c>
       <c r="I15">
         <f ca="1">RAND()*(0.7-0.35)+0.35</f>
-        <v>0.42643437867936196</v>
+        <v>0.51238375719292861</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" si="5"/>
-        <v>1.1200000000000001</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.2005100947915297</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1043,11 +1043,11 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>315486012.0996303</v>
+        <v>293855926.13184494</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" ref="C16:C25" ca="1" si="6">D16*J16</f>
-        <v>108343564.76386534</v>
+        <f t="shared" ref="C16:C26" ca="1" si="6">D16*J16</f>
+        <v>108131540.28671333</v>
       </c>
       <c r="D16">
         <v>82895775</v>
@@ -1064,15 +1064,15 @@
       </c>
       <c r="H16" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.30698536522356346</v>
+        <v>0.30442764165861691</v>
       </c>
       <c r="I16">
         <f t="shared" ref="I16:I25" ca="1" si="7">RAND()*(0.7-0.35)+0.35</f>
-        <v>0.44352258375101639</v>
+        <v>0.41311416230835929</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.3069853652235635</v>
+        <v>1.3044276416586169</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1081,11 +1081,11 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>641433143.34267211</v>
+        <v>680197977.93797779</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>416152889.10505432</v>
+        <v>401536438.54093862</v>
       </c>
       <c r="D17">
         <v>314717229</v>
@@ -1102,15 +1102,15 @@
       </c>
       <c r="H17" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.32230729924561685</v>
+        <v>0.27586417755647763</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="7"/>
-        <v>0.50208768123032266</v>
+        <v>0.53243121136630156</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.3223072992456169</v>
+        <v>1.2758641775564776</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1119,11 +1119,11 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>556412081.82920003</v>
+        <v>770651317.69935977</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>391113851.00444841</v>
+        <v>385595493.86452264</v>
       </c>
       <c r="D18">
         <v>289754271</v>
@@ -1140,15 +1140,15 @@
       </c>
       <c r="H18" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.34981220347377862</v>
+        <v>0.33076724817120162</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="7"/>
-        <v>0.44703174907789572</v>
+        <v>0.61915551033286453</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.3498122034737787</v>
+        <v>1.3307672481712016</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1157,11 +1157,11 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>510631633.75489783</v>
+        <v>549109484.02126479</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>124528818.84608179</v>
+        <v>157793160.72406778</v>
       </c>
       <c r="D19">
         <v>110232774</v>
@@ -1178,15 +1178,15 @@
       </c>
       <c r="H19" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.12968960434654217</v>
+        <v>0.43145414016404759</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="7"/>
-        <v>0.53678058316314647</v>
+        <v>0.57722884672442565</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1296896043465421</v>
+        <v>1.4314541401640475</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1195,11 +1195,11 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>341467500.191369</v>
+        <v>437082045.29778457</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>38509884.772157244</v>
+        <v>39956530.54098291</v>
       </c>
       <c r="D20">
         <v>33286617</v>
@@ -1216,15 +1216,15 @@
       </c>
       <c r="H20" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15691795210541365</v>
+        <v>0.20037823432110596</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="7"/>
-        <v>0.4241574795298434</v>
+        <v>0.54292610153926191</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1569179521054136</v>
+        <v>1.200378234321106</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1233,11 +1233,11 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>585889362.00708771</v>
+        <v>359670250.22759396</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>157268099.67072079</v>
+        <v>169469426.52630204</v>
       </c>
       <c r="D21">
         <v>131644727</v>
@@ -1254,15 +1254,15 @@
       </c>
       <c r="H21" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19464032669322762</v>
+        <v>0.28732407585380948</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="7"/>
-        <v>0.63578207990249092</v>
+        <v>0.3902987741326881</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1946403266932277</v>
+        <v>1.2873240758538094</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1271,11 +1271,11 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>410780372.40378678</v>
+        <v>421908330.59579974</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>71336778.737800315</v>
+        <v>76437677.880908012</v>
       </c>
       <c r="D22">
         <v>56024738</v>
@@ -1292,15 +1292,15 @@
       </c>
       <c r="H22" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.27330856483077737</v>
+        <v>0.3643558294000056</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="7"/>
-        <v>0.59904930288627689</v>
+        <v>0.6152774287786219</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2733085648307774</v>
+        <v>1.3643558294000055</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>510252608.17612278</v>
+        <v>420302562.32637817</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="6"/>
-        <v>269748520.65000004</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>365016598.37174022</v>
       </c>
       <c r="D23">
         <v>256903353</v>
@@ -1329,15 +1329,16 @@
         <v>0.21833895105578058</v>
       </c>
       <c r="H23" s="3">
-        <v>0.05</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.42083236403590363</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="7"/>
-        <v>0.4336573187608449</v>
+        <v>0.35720989824682531</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="5"/>
-        <v>1.05</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.4208323640359035</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1346,11 +1347,11 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>507397008.3855744</v>
+        <v>560311745.92465866</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="6"/>
-        <v>221296913.15000001</v>
+        <v>231637890.40000004</v>
       </c>
       <c r="D24">
         <v>206819545</v>
@@ -1366,15 +1367,15 @@
         <v>0.21522283273631837</v>
       </c>
       <c r="H24" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.12</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="7"/>
-        <v>0.52801306311101692</v>
+        <v>0.58307778006830702</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" si="5"/>
-        <v>1.07</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.35">
@@ -1383,11 +1384,11 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>518498812.25827289</v>
+        <v>801141632.49347126</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>166698450.64749473</v>
+        <v>172453412.46126154</v>
       </c>
       <c r="D25">
         <v>134544096</v>
@@ -1404,20 +1405,20 @@
       </c>
       <c r="H25" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23898748145362511</v>
+        <v>0.28176127818541774</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="7"/>
-        <v>0.43431533967455249</v>
+        <v>0.6710682686588465</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>1.238987481453625</v>
+        <v>1.2817612781854177</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>